<commit_message>
English version of the PM calculator added
</commit_message>
<xml_diff>
--- a/tools/PenmanMonteithCalculatorEdu.xlsx
+++ b/tools/PenmanMonteithCalculatorEdu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sherzodr\Documents\eclipse-workspace\agriclimuz\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB4D831-738F-4B66-B729-0571F3E56D98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C3C61E-92F5-4A46-9653-255A6B6CBB14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="447" activeTab="1" xr2:uid="{49EFD1A0-30FE-4D89-822D-832008CA9853}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="447" xr2:uid="{49EFD1A0-30FE-4D89-822D-832008CA9853}"/>
   </bookViews>
   <sheets>
     <sheet name="Jadval" sheetId="4" r:id="rId1"/>
@@ -1856,9 +1856,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1876,15 +1873,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1896,22 +1896,33 @@
   <dxfs count="41">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <sz val="10"/>
-        <color theme="1"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1948,7 +1959,110 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="165" formatCode="0.000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2028,6 +2142,33 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="165" formatCode="0.000"/>
       <fill>
         <patternFill patternType="solid">
@@ -2048,6 +2189,469 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="0_);\(0\)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri"/>
@@ -2102,24 +2706,11 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -2152,6 +2743,12 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2194,33 +2791,6 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2314,573 +2884,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="0.000"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="0.000"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="0_);\(0\)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2888,14 +2892,10 @@
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="10"/>
         <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3076,8 +3076,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1962151" y="1657348"/>
-          <a:ext cx="6702426" cy="509589"/>
+          <a:off x="1943100" y="1657348"/>
+          <a:ext cx="2520952" cy="509589"/>
           <a:chOff x="2205964" y="1640345"/>
           <a:chExt cx="2832101" cy="435339"/>
         </a:xfrm>
@@ -4117,7 +4117,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89D7BD22-73FB-4E37-8CAD-91A3F66EA7FA}" name="EToTable" displayName="EToTable" ref="A7:AM8" totalsRowShown="0" headerRowDxfId="0" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89D7BD22-73FB-4E37-8CAD-91A3F66EA7FA}" name="EToTable" displayName="EToTable" ref="A7:AM8" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="A7:AM8" xr:uid="{40FA6F47-45BC-4011-86C7-DB7405138E56}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4160,26 +4160,26 @@
     <filterColumn colId="38" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{55BB34F4-B6C5-485F-A788-74EBA6A46346}" name="Сана" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{0343CEB4-F964-43A1-BDB3-F2FEF6A7C729}" name="Тмин" dataDxfId="16" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{9BD57D35-89FF-4084-9359-B7214AD803FE}" name="Тмакс" dataDxfId="15" dataCellStyle="Comma"/>
-    <tableColumn id="43" xr3:uid="{D58A319A-CC23-4862-9517-A6092A1A42D7}" name="Тқуруқ" dataDxfId="6" dataCellStyle="Comma"/>
-    <tableColumn id="41" xr3:uid="{08C25DB1-EBB1-4945-A54D-EAD63D211184}" name="Тнам" dataDxfId="7" dataCellStyle="Comma"/>
-    <tableColumn id="39" xr3:uid="{7C7E8A44-B879-466A-89C1-4E05F240F519}" name="Tшудринг" dataDxfId="14" dataCellStyle="Comma"/>
-    <tableColumn id="38" xr3:uid="{F0A1A411-A0AB-4D4B-9E26-50FB9CD3266E}" name="ННмин" dataDxfId="13" dataCellStyle="Comma"/>
-    <tableColumn id="36" xr3:uid="{4B11B956-95E0-434C-90A6-17DF0322DBAC}" name="ННмакс" dataDxfId="12" dataCellStyle="Comma"/>
-    <tableColumn id="32" xr3:uid="{C6ACD81E-79A4-47AB-AFA4-85E6EC03DB8D}" name="ННўрт" dataDxfId="11" dataCellStyle="Comma"/>
-    <tableColumn id="6" xr3:uid="{41B592D5-95B1-44E5-A64B-BDDC9D6D5BCA}" name="Шамол" dataDxfId="10" dataCellStyle="Comma"/>
-    <tableColumn id="20" xr3:uid="{2ABE4840-178F-4818-A24E-0EF1AE56B41F}" name="Қуёшли соат" dataDxfId="9" dataCellStyle="Comma"/>
-    <tableColumn id="27" xr3:uid="{026FEEB6-B796-4EDB-9611-B4B15F3B7F32}" name="Радиация" dataDxfId="8" dataCellStyle="Comma"/>
-    <tableColumn id="21" xr3:uid="{A535BD23-5121-4397-AC1B-E39E70B75654}" name="Tmean" dataDxfId="39" dataCellStyle="Comma">
+    <tableColumn id="1" xr3:uid="{55BB34F4-B6C5-485F-A788-74EBA6A46346}" name="Сана" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{0343CEB4-F964-43A1-BDB3-F2FEF6A7C729}" name="Тмин" dataDxfId="37" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{9BD57D35-89FF-4084-9359-B7214AD803FE}" name="Тмакс" dataDxfId="36" dataCellStyle="Comma"/>
+    <tableColumn id="43" xr3:uid="{D58A319A-CC23-4862-9517-A6092A1A42D7}" name="Тқуруқ" dataDxfId="35" dataCellStyle="Comma"/>
+    <tableColumn id="41" xr3:uid="{08C25DB1-EBB1-4945-A54D-EAD63D211184}" name="Тнам" dataDxfId="34" dataCellStyle="Comma"/>
+    <tableColumn id="39" xr3:uid="{7C7E8A44-B879-466A-89C1-4E05F240F519}" name="Tшудринг" dataDxfId="33" dataCellStyle="Comma"/>
+    <tableColumn id="38" xr3:uid="{F0A1A411-A0AB-4D4B-9E26-50FB9CD3266E}" name="ННмин" dataDxfId="32" dataCellStyle="Comma"/>
+    <tableColumn id="36" xr3:uid="{4B11B956-95E0-434C-90A6-17DF0322DBAC}" name="ННмакс" dataDxfId="31" dataCellStyle="Comma"/>
+    <tableColumn id="32" xr3:uid="{C6ACD81E-79A4-47AB-AFA4-85E6EC03DB8D}" name="ННўрт" dataDxfId="30" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{41B592D5-95B1-44E5-A64B-BDDC9D6D5BCA}" name="Шамол" dataDxfId="29" dataCellStyle="Comma"/>
+    <tableColumn id="20" xr3:uid="{2ABE4840-178F-4818-A24E-0EF1AE56B41F}" name="Қуёшли соат" dataDxfId="28" dataCellStyle="Comma"/>
+    <tableColumn id="27" xr3:uid="{026FEEB6-B796-4EDB-9611-B4B15F3B7F32}" name="Радиация" dataDxfId="27" dataCellStyle="Comma"/>
+    <tableColumn id="21" xr3:uid="{A535BD23-5121-4397-AC1B-E39E70B75654}" name="Tmean" dataDxfId="26" dataCellStyle="Comma">
       <calculatedColumnFormula xml:space="preserve"> IF(
           AND(ISNUMBER(EToTable[[#This Row],[Сана]]), ISNUMBER(EToTable[[#This Row],[Тмин]]), ISNUMBER(EToTable[[#This Row],[Тмакс]])),
           (EToTable[[#This Row],[Тмин]]+EToTable[[#This Row],[Тмакс]])/2,
          ""
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{28F03338-A80A-46CA-90C2-3EE3FE3141B5}" name="Tdew" dataDxfId="38" dataCellStyle="Comma">
+    <tableColumn id="4" xr3:uid="{28F03338-A80A-46CA-90C2-3EE3FE3141B5}" name="Tdew" dataDxfId="25" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(
         AND(ISNUMBER(EToTable[[#This Row],[Сана]]), ISNUMBER(EToTable[[#This Row],[Тмин]]), ISNUMBER(EToTable[[#This Row],[Tшудринг]]), EToTable[[#This Row],[Tшудринг]]&lt;=EToTable[[#This Row],[Тмин]]),
          EToTable[[#This Row],[Tшудринг]],
@@ -4190,88 +4190,88 @@
          )
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{72ED62CD-F87B-4F4E-8A95-741E4046A8D2}" name="J" dataDxfId="37" dataCellStyle="Comma">
+    <tableColumn id="22" xr3:uid="{72ED62CD-F87B-4F4E-8A95-741E4046A8D2}" name="J" dataDxfId="24" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(
          ISNUMBER(EToTable[[#This Row],[Сана]]),
          _xlfn.DAYS(EToTable[[#This Row],[Сана]], "1/1/" &amp; YEAR(EToTable[[#This Row],[Сана]])) + 1,
          ""
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{91194067-8744-4547-AC20-6D98CC22490B}" name="P" dataDxfId="36" dataCellStyle="Comma">
+    <tableColumn id="34" xr3:uid="{91194067-8744-4547-AC20-6D98CC22490B}" name="P" dataDxfId="23" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(
          AND(ISNUMBER(Altitude), ISNUMBER(EToTable[[#This Row],[Сана]])),
          ROUND(101.3 * POWER( (293-0.0065 * Altitude) / 293, 5.26), 2),
         ""
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{29003213-DC54-4480-A40A-0FC6ABBE0369}" name="γ" dataDxfId="35" dataCellStyle="Comma">
+    <tableColumn id="33" xr3:uid="{29003213-DC54-4480-A40A-0FC6ABBE0369}" name="γ" dataDxfId="22" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(
         ISNUMBER(EToTable[[#This Row],[P]]),
         (Cp * EToTable[[#This Row],[P]]) / (0.622 * 2.45),
         ""
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{0E062F52-C43F-4056-A51C-394BD475D85F}" name="Δ" dataDxfId="34" dataCellStyle="Comma">
+    <tableColumn id="19" xr3:uid="{0E062F52-C43F-4056-A51C-394BD475D85F}" name="Δ" dataDxfId="21" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(
          ISNUMBER(EToTable[[#This Row],[Tmean]]),
           ROUND((4098 * (0.6108 * EXP((17.27 * EToTable[[#This Row],[Tmean]]) / (EToTable[[#This Row],[Tmean]] + 237.3)))) / ((EToTable[[#This Row],[Tmean]] + 237.3) ^ 2), 4),
          ""
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{76882BE6-D768-4B05-B6A0-08F20B3C673F}" name="δ (rad)" dataDxfId="33" dataCellStyle="Comma">
+    <tableColumn id="18" xr3:uid="{76882BE6-D768-4B05-B6A0-08F20B3C673F}" name="δ (rad)" dataDxfId="20" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(
         ISNUMBER(EToTable[[#This Row],[J]]),
         0.409  * SIN( (2*PI()/365) * EToTable[[#This Row],[J]] - 1.39),
         ""
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A21CD0BD-4854-4025-84DD-72F473757E0B}" name="dr" dataDxfId="32" dataCellStyle="Comma">
+    <tableColumn id="17" xr3:uid="{A21CD0BD-4854-4025-84DD-72F473757E0B}" name="dr" dataDxfId="19" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(
          ISNUMBER(EToTable[[#This Row],[J]]),
           ROUND(1+0.033 * COS( (2*PI()/365) * EToTable[[#This Row],[J]]), 4),
           ""
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{CE40DA70-CBFE-48A6-AC64-4663E945330A}" name="φ" dataDxfId="31" dataCellStyle="Comma">
+    <tableColumn id="23" xr3:uid="{CE40DA70-CBFE-48A6-AC64-4663E945330A}" name="φ" dataDxfId="18" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(
          AND(ISNUMBER(Latitude), ISNUMBER(EToTable[[#This Row],[Сана]])),
           ROUND((Latitude / 180) * PI(), 3),
           ""
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{F874822E-F3EF-4453-A539-2D54B0627751}" name="ωs" dataDxfId="30" dataCellStyle="Comma">
+    <tableColumn id="16" xr3:uid="{F874822E-F3EF-4453-A539-2D54B0627751}" name="ωs" dataDxfId="17" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(
         AND(ISNUMBER(EToTable[[#This Row],[φ]]), ISNUMBER(EToTable[[#This Row],[δ (rad)]])),
         ACOS( - 1 * TAN(EToTable[[#This Row],[φ]]) * TAN(EToTable[[#This Row],[δ (rad)]])),
         ""
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{8FD74915-A745-43A9-912D-0965AB100C05}" name="Ra" dataDxfId="29" dataCellStyle="Comma">
+    <tableColumn id="15" xr3:uid="{8FD74915-A745-43A9-912D-0965AB100C05}" name="Ra" dataDxfId="16" dataCellStyle="Comma">
       <calculatedColumnFormula xml:space="preserve"> IF(
          AND(ISNUMBER(EToTable[[#This Row],[ωs]]), ISNUMBER(EToTable[[#This Row],[dr]])),
          ((24 * 60) / 3.1416) * 0.082 * EToTable[[#This Row],[dr]] * ((EToTable[[#This Row],[ωs]] * SIN(EToTable[[#This Row],[φ]]) * SIN(EToTable[[#This Row],[δ (rad)]])) + (COS(EToTable[[#This Row],[φ]]) * COS(EToTable[[#This Row],[δ (rad)]]) * SIN(EToTable[[#This Row],[ωs]]))),
           ""
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{BD9990DB-8992-4E9A-893D-DCB28C028665}" name="N" dataDxfId="28" dataCellStyle="Comma">
+    <tableColumn id="14" xr3:uid="{BD9990DB-8992-4E9A-893D-DCB28C028665}" name="N" dataDxfId="15" dataCellStyle="Comma">
       <calculatedColumnFormula xml:space="preserve"> IF(ISNUMBER(EToTable[[#This Row],[ωs]]), ( 24 / PI()) * EToTable[[#This Row],[ωs]], "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{017B251A-16BB-4EF8-B942-DB81DD2D951E}" name="e° (Tmin)" dataDxfId="27" dataCellStyle="Comma">
+    <tableColumn id="13" xr3:uid="{017B251A-16BB-4EF8-B942-DB81DD2D951E}" name="e° (Tmin)" dataDxfId="14" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(ISNUMBER(EToTable[[#This Row],[Тмин]]), 0.6108 * EXP( 17.27 * EToTable[[#This Row],[Тмин]] / (EToTable[[#This Row],[Тмин]]+237.3)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{0488585F-8BE0-4299-A580-08C3CBFA1E59}" name="e° (Tmax)" dataDxfId="26" dataCellStyle="Comma">
+    <tableColumn id="12" xr3:uid="{0488585F-8BE0-4299-A580-08C3CBFA1E59}" name="e° (Tmax)" dataDxfId="13" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(ISNUMBER(EToTable[[#This Row],[Тмакс]]), 0.6108 * EXP( 17.27 * EToTable[[#This Row],[Тмакс]] / (EToTable[[#This Row],[Тмакс]]+237.3)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="44" xr3:uid="{0DE5F26D-7C9B-4663-BE84-113862C060B3}" name="e° (Twet)" dataDxfId="5" dataCellStyle="Comma">
+    <tableColumn id="44" xr3:uid="{0DE5F26D-7C9B-4663-BE84-113862C060B3}" name="e° (Twet)" dataDxfId="12" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(AND(ISNUMBER(EToTable[[#This Row],[Тнам]]), ISNUMBER(EToTable[[#This Row],[Тқуруқ]]), ISNUMBER(EToTable[[#This Row],[P]])),  0.6108 * EXP( 17.27 * EToTable[[#This Row],[Тнам]] / (EToTable[[#This Row],[Тнам]]+237.3)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{DC14E8C3-BA59-4195-BBB3-8106DA52F7F7}" name="es" dataDxfId="4" dataCellStyle="Comma">
+    <tableColumn id="11" xr3:uid="{DC14E8C3-BA59-4195-BBB3-8106DA52F7F7}" name="es" dataDxfId="11" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(AND(ISNUMBER(EToTable[[#This Row],[e° (Tmin)]]), ISNUMBER(EToTable[[#This Row],[e° (Tmax)]])), (EToTable[[#This Row],[e° (Tmax)]]+EToTable[[#This Row],[e° (Tmin)]])/2, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{57F5EDAF-2374-49FE-9B64-AB6BBD822583}" name="e° (Tdew)" dataDxfId="2" dataCellStyle="Comma">
+    <tableColumn id="24" xr3:uid="{57F5EDAF-2374-49FE-9B64-AB6BBD822583}" name="e° (Tdew)" dataDxfId="10" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(ISNUMBER(EToTable[[#This Row],[Tdew]]), 0.6108 * EXP( 17.27 * (EToTable[[#This Row],[Tdew]]) / (EToTable[[#This Row],[Tdew]]+237.3)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{627FA355-70D4-4E6A-A764-1C5826BB96A2}" name="ea" dataDxfId="3" dataCellStyle="Comma">
+    <tableColumn id="10" xr3:uid="{627FA355-70D4-4E6A-A764-1C5826BB96A2}" name="ea" dataDxfId="9" dataCellStyle="Comma">
       <calculatedColumnFormula xml:space="preserve"> IF(
         ISNUMBER(EToTable[[#This Row],[Tшудринг]]),
         EToTable[[#This Row],[e° (Tdew)]],
@@ -4298,13 +4298,13 @@
       )
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9E010230-CD5B-42D5-8FA2-D17763D5D2AC}" name="es - ea" dataDxfId="25" dataCellStyle="Comma">
+    <tableColumn id="9" xr3:uid="{9E010230-CD5B-42D5-8FA2-D17763D5D2AC}" name="es - ea" dataDxfId="8" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(AND(ISNUMBER(EToTable[[#This Row],[es]]), ISNUMBER(EToTable[[#This Row],[ea]])), EToTable[[#This Row],[es]]-EToTable[[#This Row],[ea]], "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{5EAFCF03-F1FE-46B0-8665-1FD5A41B6C5E}" name="Rso" dataDxfId="24" dataCellStyle="Comma">
+    <tableColumn id="8" xr3:uid="{5EAFCF03-F1FE-46B0-8665-1FD5A41B6C5E}" name="Rso" dataDxfId="7" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(ISNUMBER(EToTable[[#This Row],[Ra]]), (as+bs)*EToTable[[#This Row],[Ra]], "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{42FE00EA-A686-4C84-8B12-E62382B4D2E8}" name="Rs" dataDxfId="23" dataCellStyle="Comma">
+    <tableColumn id="26" xr3:uid="{42FE00EA-A686-4C84-8B12-E62382B4D2E8}" name="Rs" dataDxfId="6" dataCellStyle="Comma">
       <calculatedColumnFormula xml:space="preserve"> IF(
         ISNUMBER(EToTable[[#This Row],[Радиация]]),
         EToTable[[#This Row],[Радиация]],
@@ -4319,32 +4319,32 @@
        )
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{D2310C7E-B446-4405-BEDC-9493BA3EA074}" name="Rns" dataDxfId="22" dataCellStyle="Comma">
+    <tableColumn id="25" xr3:uid="{D2310C7E-B446-4405-BEDC-9493BA3EA074}" name="Rns" dataDxfId="5" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(ISNUMBER(EToTable[[#This Row],[Rs]]), (1-albedo)*EToTable[[#This Row],[Rs]], "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{246D79AE-5292-4B8C-8FD4-BAB9ABA083D4}" name="Rnl" dataDxfId="21" dataCellStyle="Comma">
+    <tableColumn id="28" xr3:uid="{246D79AE-5292-4B8C-8FD4-BAB9ABA083D4}" name="Rnl" dataDxfId="4" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(AND(ISNUMBER(EToTable[[#This Row],[Rso]]), ISNUMBER(EToTable[[#This Row],[ea]]), ISNUMBER(EToTable[[#This Row],[Rs]])), StefanBoltzmann *
 (( POWER(EToTable[[#This Row],[Тмакс]]+273.16, 4) + POWER( EToTable[[#This Row],[Тмин]]+273.16, 4) ) / 2 ) *
 (0.34 - 0.14 * SQRT(EToTable[[#This Row],[ea]])) *
 ( (1.35 * EToTable[[#This Row],[Rs]]/EToTable[[#This Row],[Rso]]) - 0.35), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{422888C5-5DC5-4D70-B7D8-B3F6A9456433}" name="Rn" dataDxfId="20" dataCellStyle="Comma">
+    <tableColumn id="29" xr3:uid="{422888C5-5DC5-4D70-B7D8-B3F6A9456433}" name="Rn" dataDxfId="3" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(AND(ISNUMBER(EToTable[[#This Row],[Rns]]), ISNUMBER(EToTable[[#This Row],[Rnl]])), EToTable[[#This Row],[Rns]]-EToTable[[#This Row],[Rnl]], "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{9B0CC101-DA7D-4460-9098-E50E3E62164F}" name="u2" dataDxfId="19" dataCellStyle="Comma">
+    <tableColumn id="30" xr3:uid="{9B0CC101-DA7D-4460-9098-E50E3E62164F}" name="u2" dataDxfId="2" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(AND(ISNUMBER(EToTable[[#This Row],[Сана]]), ISNUMBER(AnemometerHeight)), IF(ISNUMBER(EToTable[[#This Row],[Шамол]]),
      IF(AnemometerHeight=2, MAX(EToTable[[#This Row],[Шамол]], 0.5),
      MAX( EToTable[[#This Row],[Шамол]] * 4.87 / LN(67.8 * AnemometerHeight - 5.42), 0.5)
 ), u2_default), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{F7425A71-C167-48A6-930B-0E92D3200E4B}" name=" ETO  (ФАО)" dataDxfId="18" dataCellStyle="Comma">
+    <tableColumn id="7" xr3:uid="{F7425A71-C167-48A6-930B-0E92D3200E4B}" name=" ETO  (ФАО)" dataDxfId="1" dataCellStyle="Comma">
       <calculatedColumnFormula xml:space="preserve"> IF(
            AND(ISNUMBER(Latitude), ISNUMBER(Altitude), ISNUMBER(EToTable[[#This Row],[Сана]]), ISNUMBER(EToTable[[#This Row],[Тмин]]), ISNUMBER(EToTable[[#This Row],[Тмакс]])),
            ((0.408 * EToTable[[#This Row],[Δ]] * (EToTable[[#This Row],[Rn]]-0))   + EToTable[[#This Row],[γ]] * (900 / (EToTable[[#This Row],[Tmean]]+273) ) * MAX( EToTable[[#This Row],[u2]], 0.5) * EToTable[[#This Row],[es - ea]]) / (EToTable[[#This Row],[Δ]]  + EToTable[[#This Row],[γ]]*(1+0.34 * MAX(EToTable[[#This Row],[u2]], 0.5))),
            ""
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="45" xr3:uid="{5F0ADAD7-889F-48DD-A4BC-ABB7440E092B}" name="ЕТО_x000a_ (Харгривс)" dataDxfId="1" dataCellStyle="Comma">
+    <tableColumn id="45" xr3:uid="{5F0ADAD7-889F-48DD-A4BC-ABB7440E092B}" name="ЕТО_x000a_ (Харгривс)" dataDxfId="0" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(
            ISNUMBER(EToTable[[#This Row],[ ETO  (ФАО)]]),
            0.0023 * (EToTable[[#This Row],[Tmean]]+17.8) * SQRT(EToTable[[#This Row],[Тмакс]]-EToTable[[#This Row],[Тмин]])*EToTable[[#This Row],[Ra]] * 0.408,
@@ -4656,25 +4656,26 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AP8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="9.7109375" style="1" customWidth="1"/>
-    <col min="4" max="6" width="9.7109375" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="9" width="11.28515625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="12.42578125" style="1" customWidth="1"/>
+    <col min="4" max="6" width="9.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="9" width="11.28515625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="12.42578125" style="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="14.140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="11.28515625" style="1" customWidth="1"/>
-    <col min="13" max="37" width="7.7109375" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="39" width="10.28515625" style="1" customWidth="1"/>
+    <col min="13" max="37" width="7.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="10.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="10.28515625" style="1" customWidth="1"/>
     <col min="40" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="52" t="s">
         <v>43</v>
       </c>
       <c r="B1" s="36"/>
@@ -4717,9 +4718,9 @@
       <c r="AM1" s="3"/>
     </row>
     <row r="2" spans="1:42" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
+      <c r="A2" s="56"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
       <c r="F2" s="37"/>
@@ -4727,10 +4728,10 @@
       <c r="H2" s="37"/>
       <c r="I2" s="37"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="51" t="s">
+      <c r="K2" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="50"/>
+      <c r="L2" s="49"/>
       <c r="M2" s="37"/>
       <c r="N2" s="37"/>
       <c r="O2" s="37"/>
@@ -4801,11 +4802,11 @@
       <c r="AM3" s="3"/>
     </row>
     <row r="4" spans="1:42" ht="30.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="49"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="48"/>
       <c r="D4" s="37"/>
       <c r="E4" s="37"/>
       <c r="F4" s="37"/>
@@ -4813,10 +4814,10 @@
       <c r="H4" s="40"/>
       <c r="I4" s="40"/>
       <c r="J4" s="3"/>
-      <c r="K4" s="52" t="s">
+      <c r="K4" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="50">
+      <c r="L4" s="49">
         <v>2</v>
       </c>
       <c r="M4" s="36"/>
@@ -4910,22 +4911,22 @@
       <c r="C7" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="48" t="s">
+      <c r="F7" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="48" t="s">
+      <c r="G7" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="48" t="s">
+      <c r="H7" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="48" t="s">
+      <c r="I7" s="47" t="s">
         <v>38</v>
       </c>
       <c r="J7" s="44" t="s">
@@ -4937,79 +4938,79 @@
       <c r="L7" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="M7" s="56" t="s">
+      <c r="M7" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="N7" s="56" t="s">
+      <c r="N7" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="O7" s="56" t="s">
+      <c r="O7" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="P7" s="56" t="s">
+      <c r="P7" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="Q7" s="56" t="s">
+      <c r="Q7" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="R7" s="56" t="s">
+      <c r="R7" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S7" s="56" t="s">
+      <c r="S7" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="T7" s="56" t="s">
+      <c r="T7" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="U7" s="56" t="s">
+      <c r="U7" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="V7" s="56" t="s">
+      <c r="V7" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="W7" s="56" t="s">
+      <c r="W7" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="X7" s="56" t="s">
+      <c r="X7" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="Y7" s="56" t="s">
+      <c r="Y7" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="Z7" s="56" t="s">
+      <c r="Z7" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="AA7" s="56" t="s">
+      <c r="AA7" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="AB7" s="56" t="s">
+      <c r="AB7" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="AC7" s="56" t="s">
+      <c r="AC7" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="AD7" s="56" t="s">
+      <c r="AD7" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="AE7" s="56" t="s">
+      <c r="AE7" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="AF7" s="56" t="s">
+      <c r="AF7" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="AG7" s="56" t="s">
+      <c r="AG7" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="AH7" s="56" t="s">
+      <c r="AH7" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="AI7" s="56" t="s">
+      <c r="AI7" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="AJ7" s="56" t="s">
+      <c r="AJ7" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="AK7" s="56" t="s">
+      <c r="AK7" s="53" t="s">
         <v>62</v>
       </c>
       <c r="AL7" s="45" t="s">
@@ -5298,7 +5299,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>

</xml_diff>